<commit_message>
Excel Database file (please do not remake this file)
</commit_message>
<xml_diff>
--- a/Code Part/Taxi-information.xlsx
+++ b/Code Part/Taxi-information.xlsx
@@ -8,39 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dangd\Documents\USTH\2nd year\Advanced Programming with Python\Taxi-Information-Management-System-\Code Part\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB5F1DD-A6C5-4A64-80C9-882CDB47936F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E9E42F-7B3B-4FB5-8C9B-77C6E471C0D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer" sheetId="1" r:id="rId1"/>
     <sheet name="Driver" sheetId="2" r:id="rId2"/>
-    <sheet name="Vehicle" sheetId="3" r:id="rId3"/>
-    <sheet name="Invoice" sheetId="4" r:id="rId4"/>
-    <sheet name="Price per Km" sheetId="5" r:id="rId5"/>
+    <sheet name="Vehicle" sheetId="4" r:id="rId3"/>
+    <sheet name="Invoice" sheetId="5" r:id="rId4"/>
+    <sheet name="Price per Km" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="129">
   <si>
     <t>id</t>
   </si>
@@ -57,60 +41,90 @@
     <t>Obama</t>
   </si>
   <si>
+    <t>0990154927</t>
+  </si>
+  <si>
     <t>C2</t>
   </si>
   <si>
     <t>Trump</t>
   </si>
   <si>
+    <t>0994586705</t>
+  </si>
+  <si>
     <t>C3</t>
   </si>
   <si>
     <t>Lincole</t>
   </si>
   <si>
+    <t>0993224669</t>
+  </si>
+  <si>
     <t>C4</t>
   </si>
   <si>
     <t>Wasington</t>
   </si>
   <si>
+    <t>0992006894</t>
+  </si>
+  <si>
     <t>C5</t>
   </si>
   <si>
     <t>Machiel</t>
   </si>
   <si>
+    <t>0995267883</t>
+  </si>
+  <si>
     <t>C6</t>
   </si>
   <si>
     <t>Kalanith</t>
   </si>
   <si>
+    <t>0992111784</t>
+  </si>
+  <si>
     <t>C7</t>
   </si>
   <si>
     <t>Jack</t>
   </si>
   <si>
+    <t>0999469153</t>
+  </si>
+  <si>
     <t>C8</t>
   </si>
   <si>
     <t>London</t>
   </si>
   <si>
+    <t>0995597996</t>
+  </si>
+  <si>
     <t>C9</t>
   </si>
   <si>
     <t>Francais</t>
   </si>
   <si>
+    <t>0994908696</t>
+  </si>
+  <si>
     <t>C10</t>
   </si>
   <si>
     <t>Martel</t>
   </si>
   <si>
+    <t>0990811244</t>
+  </si>
+  <si>
     <t>vehicle_id</t>
   </si>
   <si>
@@ -129,6 +143,9 @@
     <t>Bob</t>
   </si>
   <si>
+    <t>0994109078</t>
+  </si>
+  <si>
     <t>5S123</t>
   </si>
   <si>
@@ -141,6 +158,9 @@
     <t>James</t>
   </si>
   <si>
+    <t>0996231061</t>
+  </si>
+  <si>
     <t>9S321</t>
   </si>
   <si>
@@ -150,6 +170,9 @@
     <t>Charle</t>
   </si>
   <si>
+    <t>0991555385</t>
+  </si>
+  <si>
     <t>7S444</t>
   </si>
   <si>
@@ -162,6 +185,9 @@
     <t>Max</t>
   </si>
   <si>
+    <t>0990737267</t>
+  </si>
+  <si>
     <t>5S322</t>
   </si>
   <si>
@@ -171,6 +197,9 @@
     <t>Chris</t>
   </si>
   <si>
+    <t>0990454930</t>
+  </si>
+  <si>
     <t>5S111</t>
   </si>
   <si>
@@ -180,6 +209,9 @@
     <t>Mark</t>
   </si>
   <si>
+    <t>0997945252</t>
+  </si>
+  <si>
     <t>7S333</t>
   </si>
   <si>
@@ -189,6 +221,9 @@
     <t>Joey</t>
   </si>
   <si>
+    <t>0999800731</t>
+  </si>
+  <si>
     <t>7S932</t>
   </si>
   <si>
@@ -198,6 +233,9 @@
     <t>Paul</t>
   </si>
   <si>
+    <t>0992376425</t>
+  </si>
+  <si>
     <t>9S233</t>
   </si>
   <si>
@@ -207,6 +245,9 @@
     <t>Eric</t>
   </si>
   <si>
+    <t>0995920106</t>
+  </si>
+  <si>
     <t>9S193</t>
   </si>
   <si>
@@ -216,6 +257,9 @@
     <t>Barker</t>
   </si>
   <si>
+    <t>0996309582</t>
+  </si>
+  <si>
     <t>5S094</t>
   </si>
   <si>
@@ -228,6 +272,45 @@
     <t>price</t>
   </si>
   <si>
+    <t>5S</t>
+  </si>
+  <si>
+    <t>29-B1 423.23</t>
+  </si>
+  <si>
+    <t>9S</t>
+  </si>
+  <si>
+    <t>29-C1 312.93</t>
+  </si>
+  <si>
+    <t>7S</t>
+  </si>
+  <si>
+    <t>29-D1 123.32</t>
+  </si>
+  <si>
+    <t>29-B2 445.63</t>
+  </si>
+  <si>
+    <t>29-C2 278.42</t>
+  </si>
+  <si>
+    <t>29-D2 444.44</t>
+  </si>
+  <si>
+    <t>29-B3 888.88</t>
+  </si>
+  <si>
+    <t>29-C3 999.99</t>
+  </si>
+  <si>
+    <t>29-D3 100.00</t>
+  </si>
+  <si>
+    <t>29-B4 344.44</t>
+  </si>
+  <si>
     <t>customer_id</t>
   </si>
   <si>
@@ -300,104 +383,43 @@
     <t>9s</t>
   </si>
   <si>
-    <t>29-B1 423.23</t>
-  </si>
-  <si>
-    <t>29-C1 312.93</t>
-  </si>
-  <si>
-    <t>29-D1 123.32</t>
-  </si>
-  <si>
-    <t>29-B2 445.63</t>
-  </si>
-  <si>
-    <t>29-C2 278.42</t>
-  </si>
-  <si>
-    <t>29-D2 444.44</t>
-  </si>
-  <si>
-    <t>29-B3 888.88</t>
-  </si>
-  <si>
-    <t>29-C3 999.99</t>
-  </si>
-  <si>
-    <t>29-D3 100.00</t>
-  </si>
-  <si>
-    <t>29-B4 344.44</t>
-  </si>
-  <si>
-    <t>0994109078</t>
-  </si>
-  <si>
-    <t>0996231061</t>
-  </si>
-  <si>
-    <t>0991555385</t>
-  </si>
-  <si>
-    <t>0990737267</t>
-  </si>
-  <si>
-    <t>0990454930</t>
-  </si>
-  <si>
-    <t>0997945252</t>
-  </si>
-  <si>
-    <t>0999800731</t>
-  </si>
-  <si>
-    <t>0992376425</t>
-  </si>
-  <si>
-    <t>0995920106</t>
-  </si>
-  <si>
-    <t>0996309582</t>
-  </si>
-  <si>
-    <t>0990154927</t>
-  </si>
-  <si>
-    <t>0994586705</t>
-  </si>
-  <si>
-    <t>0993224669</t>
-  </si>
-  <si>
-    <t>0992006894</t>
-  </si>
-  <si>
-    <t>0995267883</t>
-  </si>
-  <si>
-    <t>0992111784</t>
-  </si>
-  <si>
-    <t>0999469153</t>
-  </si>
-  <si>
-    <t>0995597996</t>
-  </si>
-  <si>
-    <t>0994908696</t>
-  </si>
-  <si>
-    <t>0990811244</t>
+    <t>2022-07-28</t>
+  </si>
+  <si>
+    <t>2022-10-21</t>
+  </si>
+  <si>
+    <t>2022-07-22</t>
+  </si>
+  <si>
+    <t>2022-12-15</t>
+  </si>
+  <si>
+    <t>2022-10-01</t>
+  </si>
+  <si>
+    <t>2022-08-20</t>
+  </si>
+  <si>
+    <t>2022-04-08</t>
+  </si>
+  <si>
+    <t>2022-07-08</t>
+  </si>
+  <si>
+    <t>2023-02-05</t>
+  </si>
+  <si>
+    <t>2022-07-26</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="165" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="#,##0;[Red]#,##0"/>
-    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd;@"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="#,##0;[Red]#,##0"/>
+    <numFmt numFmtId="166" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -448,21 +470,22 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -781,7 +804,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -810,106 +833,106 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>106</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>107</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>108</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>109</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>110</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>111</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>112</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>113</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>114</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>115</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -923,7 +946,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -944,36 +967,36 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>96</v>
+        <v>39</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E2" s="3">
         <v>15000000</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="G2" s="4">
         <v>18</v>
@@ -981,22 +1004,22 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>97</v>
+        <v>44</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="E3" s="3">
         <v>12000000</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="G3" s="4">
         <v>30</v>
@@ -1004,22 +1027,22 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>98</v>
+        <v>48</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="E4" s="3">
         <v>14000000</v>
       </c>
       <c r="F4" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="G4" s="4">
         <v>64</v>
@@ -1027,22 +1050,22 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>99</v>
+        <v>53</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="E5" s="3">
         <v>15000000</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="G5" s="4">
         <v>28</v>
@@ -1050,22 +1073,22 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>100</v>
+        <v>57</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="E6" s="3">
         <v>17000000</v>
       </c>
       <c r="F6" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="G6" s="4">
         <v>34</v>
@@ -1073,22 +1096,22 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>101</v>
+        <v>61</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="E7" s="3">
         <v>17000000</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="G7" s="4">
         <v>27</v>
@@ -1096,22 +1119,22 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>102</v>
+        <v>65</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="E8" s="3">
         <v>20000000</v>
       </c>
       <c r="F8" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="G8" s="4">
         <v>49</v>
@@ -1119,22 +1142,22 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>103</v>
+        <v>69</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="E9" s="3">
         <v>19000000</v>
       </c>
       <c r="F9" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="G9" s="4">
         <v>44</v>
@@ -1142,22 +1165,22 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>104</v>
+        <v>73</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="E10" s="3">
         <v>19000000</v>
       </c>
       <c r="F10" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="G10" s="4">
         <v>42</v>
@@ -1165,22 +1188,22 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>105</v>
+        <v>77</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="E11" s="3">
         <v>16000000</v>
       </c>
       <c r="F11" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="G11" s="4">
         <v>23</v>
@@ -1188,15 +1211,15 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -1210,172 +1233,152 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" t="str">
-        <f t="shared" ref="B2:B11" si="0">LEFT(A2,2)</f>
-        <v>5S</v>
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>82</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D2" s="5">
-        <f>VLOOKUP(B2, 'Price per Km'!$A$2:$B$4,2,0)</f>
         <v>10000</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" t="str">
-        <f t="shared" si="0"/>
-        <v>9S</v>
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
+        <v>84</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D3" s="5">
-        <f>VLOOKUP(B3, 'Price per Km'!$A$2:$B$4,2,0)</f>
         <v>15000</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" t="str">
-        <f t="shared" si="0"/>
-        <v>7S</v>
+        <v>49</v>
+      </c>
+      <c r="B4" t="s">
+        <v>86</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D4" s="5">
-        <f>VLOOKUP(B4, 'Price per Km'!$A$2:$B$4,2,0)</f>
         <v>13000</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" t="str">
-        <f t="shared" si="0"/>
-        <v>5S</v>
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
+        <v>82</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D5" s="5">
-        <f>VLOOKUP(B5, 'Price per Km'!$A$2:$B$4,2,0)</f>
         <v>10000</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" t="str">
-        <f t="shared" si="0"/>
-        <v>5S</v>
+        <v>58</v>
+      </c>
+      <c r="B6" t="s">
+        <v>82</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D6" s="5">
-        <f>VLOOKUP(B6, 'Price per Km'!$A$2:$B$4,2,0)</f>
         <v>10000</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" t="str">
-        <f t="shared" si="0"/>
-        <v>7S</v>
+        <v>62</v>
+      </c>
+      <c r="B7" t="s">
+        <v>86</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D7" s="5">
-        <f>VLOOKUP(B7, 'Price per Km'!$A$2:$B$4,2,0)</f>
         <v>13000</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" t="str">
-        <f t="shared" si="0"/>
-        <v>7S</v>
+        <v>66</v>
+      </c>
+      <c r="B8" t="s">
+        <v>86</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D8" s="5">
-        <f>VLOOKUP(B8, 'Price per Km'!$A$2:$B$4,2,0)</f>
         <v>13000</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9" t="str">
-        <f t="shared" si="0"/>
-        <v>9S</v>
+        <v>70</v>
+      </c>
+      <c r="B9" t="s">
+        <v>84</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D9" s="5">
-        <f>VLOOKUP(B9, 'Price per Km'!$A$2:$B$4,2,0)</f>
         <v>15000</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B10" t="str">
-        <f t="shared" si="0"/>
-        <v>9S</v>
+        <v>74</v>
+      </c>
+      <c r="B10" t="s">
+        <v>84</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D10" s="5">
-        <f>VLOOKUP(B10, 'Price per Km'!$A$2:$B$4,2,0)</f>
         <v>15000</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" t="str">
-        <f t="shared" si="0"/>
-        <v>5S</v>
+        <v>78</v>
+      </c>
+      <c r="B11" t="s">
+        <v>82</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D11" s="5">
-        <f>VLOOKUP(B11, 'Price per Km'!$A$2:$B$4,2,0)</f>
         <v>10000</v>
       </c>
     </row>
@@ -1386,11 +1389,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -1398,7 +1401,7 @@
     <col min="1" max="1" width="4.28515625" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="7" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" customWidth="1"/>
     <col min="6" max="6" width="9.42578125" customWidth="1"/>
     <col min="7" max="7" width="12.28515625" customWidth="1"/>
@@ -1411,44 +1414,42 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>95</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>64</v>
+        <v>96</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>97</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>66</v>
+        <v>99</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>67</v>
+        <v>100</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B2" t="str">
-        <f>Customer!A2</f>
-        <v>C1</v>
-      </c>
-      <c r="C2" t="str">
-        <f>Driver!A2</f>
-        <v>D1</v>
-      </c>
-      <c r="D2" s="6">
-        <v>45061</v>
+        <v>102</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>119</v>
       </c>
       <c r="E2" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
       <c r="F2">
         <v>3</v>
@@ -1456,86 +1457,77 @@
       <c r="G2" s="5">
         <v>10000</v>
       </c>
-      <c r="H2" s="7">
-        <f t="shared" ref="H2:H11" si="0">F2*G2</f>
+      <c r="H2" s="6">
         <v>30000</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B3" t="str">
-        <f>Customer!A3</f>
-        <v>C2</v>
-      </c>
-      <c r="C3" t="str">
-        <f>Driver!A3</f>
-        <v>D2</v>
-      </c>
-      <c r="D3" s="6">
-        <v>45062</v>
+        <v>104</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="E3" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="F3">
         <v>8</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="6">
         <v>15000</v>
       </c>
-      <c r="H3" s="7">
-        <f t="shared" si="0"/>
+      <c r="H3" s="6">
         <v>120000</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B4" t="str">
-        <f>Customer!A4</f>
-        <v>C3</v>
-      </c>
-      <c r="C4" t="str">
-        <f>Driver!A4</f>
-        <v>D3</v>
-      </c>
-      <c r="D4" s="6">
-        <v>45103</v>
+        <v>106</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="E4" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="F4">
         <v>11</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="6">
         <v>13000</v>
       </c>
-      <c r="H4" s="7">
-        <f t="shared" si="0"/>
+      <c r="H4" s="6">
         <v>143000</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B5" t="str">
-        <f>Customer!A5</f>
-        <v>C4</v>
-      </c>
-      <c r="C5" t="str">
-        <f>Driver!A5</f>
-        <v>D4</v>
-      </c>
-      <c r="D5" s="6">
-        <v>45210</v>
+        <v>107</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>122</v>
       </c>
       <c r="E5" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
       <c r="F5">
         <v>20</v>
@@ -1543,28 +1535,25 @@
       <c r="G5" s="5">
         <v>10000</v>
       </c>
-      <c r="H5" s="7">
-        <f t="shared" si="0"/>
+      <c r="H5" s="6">
         <v>200000</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B6" t="str">
-        <f>Customer!A6</f>
-        <v>C5</v>
-      </c>
-      <c r="C6" t="str">
-        <f>Driver!A6</f>
-        <v>D5</v>
-      </c>
-      <c r="D6" s="6">
-        <v>45243</v>
+        <v>108</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>123</v>
       </c>
       <c r="E6" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="F6">
         <v>16</v>
@@ -1572,144 +1561,129 @@
       <c r="G6" s="5">
         <v>10000</v>
       </c>
-      <c r="H6" s="7">
-        <f t="shared" si="0"/>
+      <c r="H6" s="6">
         <v>160000</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B7" t="str">
-        <f>Customer!A7</f>
-        <v>C6</v>
-      </c>
-      <c r="C7" t="str">
-        <f>Driver!A7</f>
-        <v>D6</v>
-      </c>
-      <c r="D7" s="6">
-        <v>45132</v>
+        <v>109</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>124</v>
       </c>
       <c r="E7" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
       <c r="F7">
         <v>21</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="6">
         <v>13000</v>
       </c>
-      <c r="H7" s="7">
-        <f t="shared" si="0"/>
+      <c r="H7" s="6">
         <v>273000</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>77</v>
-      </c>
-      <c r="B8" t="str">
-        <f>Customer!A8</f>
-        <v>C7</v>
-      </c>
-      <c r="C8" t="str">
-        <f>Driver!A8</f>
-        <v>D7</v>
-      </c>
-      <c r="D8" s="6">
-        <v>45203</v>
+        <v>110</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>125</v>
       </c>
       <c r="E8" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
       <c r="F8">
         <v>17</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="6">
         <v>13000</v>
       </c>
-      <c r="H8" s="7">
-        <f t="shared" si="0"/>
+      <c r="H8" s="6">
         <v>221000</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B9" t="str">
-        <f>Customer!A9</f>
-        <v>C8</v>
-      </c>
-      <c r="C9" t="str">
-        <f>Driver!A9</f>
-        <v>D8</v>
-      </c>
-      <c r="D9" s="6">
-        <v>45216</v>
+        <v>111</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>126</v>
       </c>
       <c r="E9" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="F9">
         <v>7</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="6">
         <v>15000</v>
       </c>
-      <c r="H9" s="7">
-        <f t="shared" si="0"/>
+      <c r="H9" s="6">
         <v>105000</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>79</v>
-      </c>
-      <c r="B10" t="str">
-        <f>Customer!A10</f>
-        <v>C9</v>
-      </c>
-      <c r="C10" t="str">
-        <f>Driver!A10</f>
-        <v>D9</v>
-      </c>
-      <c r="D10" s="6">
-        <v>45237</v>
+        <v>112</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="E10" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
       <c r="F10">
         <v>6</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="6">
         <v>15000</v>
       </c>
-      <c r="H10" s="7">
-        <f t="shared" si="0"/>
+      <c r="H10" s="6">
         <v>90000</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>80</v>
-      </c>
-      <c r="B11" t="str">
-        <f>Customer!A11</f>
-        <v>C10</v>
-      </c>
-      <c r="C11" t="str">
-        <f>Driver!A11</f>
-        <v>D10</v>
-      </c>
-      <c r="D11" s="6">
-        <v>45263</v>
+        <v>113</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="E11" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="F11">
         <v>3</v>
@@ -1717,19 +1691,18 @@
       <c r="G11" s="5">
         <v>10000</v>
       </c>
-      <c r="H11" s="7">
-        <f t="shared" si="0"/>
+      <c r="H11" s="6">
         <v>30000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -1744,33 +1717,33 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>81</v>
+        <v>114</v>
       </c>
       <c r="B1" t="s">
-        <v>82</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B2" s="7">
+        <v>116</v>
+      </c>
+      <c r="B2" s="6">
         <v>10000</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B3" s="7">
+        <v>117</v>
+      </c>
+      <c r="B3" s="6">
         <v>13000</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B4" s="7">
+        <v>118</v>
+      </c>
+      <c r="B4" s="6">
         <v>15000</v>
       </c>
     </row>

</xml_diff>